<commit_message>
converting URIs into w3id.org/italia/controlled-vocabulary for life event, business event, service input and output controlled vocabularies and inserted German translations; added CSV and XLSX formats for business-event and life-event controlled vocabularies
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-public-services/service-input-output/service-input-output.xlsx
+++ b/VocabolariControllati/classifications-for-public-services/service-input-output/service-input-output.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Istanza/richiesta</t>
   </si>
@@ -39,15 +39,6 @@
     <t>Certificazione</t>
   </si>
   <si>
-    <t>Codice (e.g., codice microchip, altro tipo di codice)</t>
-  </si>
-  <si>
-    <t>Codice 1 livello</t>
-  </si>
-  <si>
-    <t>Label 1 livello</t>
-  </si>
-  <si>
     <t>CODE</t>
   </si>
   <si>
@@ -72,19 +63,83 @@
     <t>CERT</t>
   </si>
   <si>
-    <t>Attestazione di identità (e.g., carta di identità, tessera sanitaria, codice fiscale)</t>
+    <t xml:space="preserve">Attestazione di identità </t>
+  </si>
+  <si>
+    <t>Codice</t>
+  </si>
+  <si>
+    <t>Request/application</t>
+  </si>
+  <si>
+    <t>Gesuch / Anfrage</t>
+  </si>
+  <si>
+    <t>Other documents</t>
+  </si>
+  <si>
+    <t>Sonstige Dokumentation</t>
+  </si>
+  <si>
+    <t>Payment declaration</t>
+  </si>
+  <si>
+    <t>Zahlungsbestätigung</t>
+  </si>
+  <si>
+    <t>Authorization Act</t>
+  </si>
+  <si>
+    <t>Bewilligungsurkunde</t>
+  </si>
+  <si>
+    <t>Identity Declaration</t>
+  </si>
+  <si>
+    <t>Identitätsnachweis</t>
+  </si>
+  <si>
+    <t>Administrative documentation</t>
+  </si>
+  <si>
+    <t>Verwaltungsdokumentation</t>
+  </si>
+  <si>
+    <t>Certification</t>
+  </si>
+  <si>
+    <t>Bescheinigung</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Kode</t>
+  </si>
+  <si>
+    <t>codice _1_livello</t>
+  </si>
+  <si>
+    <t>label_ITA_1_livello</t>
+  </si>
+  <si>
+    <t>label_ENG_1_livello</t>
+  </si>
+  <si>
+    <t>label_DEU_1_livello</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -93,6 +148,11 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -116,9 +176,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -450,88 +511,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
     <col min="2" max="2" width="66.83203125" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>